<commit_message>
Clean up unit test code for warning if there are ISTD that is indicated in the Transition_Name_ISTD column but are not present in the input data.
</commit_message>
<xml_diff>
--- a/tests/testdata/test_transition_annot/WideTableForm_Annotation_ISTD_not_in_InputData_MultipleISTD.xlsx
+++ b/tests/testdata/test_transition_annot/WideTableForm_Annotation_ISTD_not_in_InputData_MultipleISTD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSOrganiser\tests\testdata\test_transition_annot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED6ACA-35EB-42EE-A5BB-AC82603CAACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EC8B7A-B495-4F0D-8966-63BB9B8BB93C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="8775" xr2:uid="{99D2A2AC-8431-4E91-B3F6-6736E2B6E0B0}"/>
   </bookViews>
@@ -631,9 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4803233F-B712-4161-B593-AE755CB87014}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>